<commit_message>
Jogar concluido, faltando melhoris visuais
</commit_message>
<xml_diff>
--- a/campo.xlsx
+++ b/campo.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="config" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="jogo" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,10 +447,8 @@
           <t>linha</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="B1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -458,10 +457,8 @@
           <t>coluna</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="B2" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -470,9 +467,157 @@
           <t>dificuldade</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>